<commit_message>
Work Activities Vertical view completed
</commit_message>
<xml_diff>
--- a/public/Daily Report_hyunmyung.kim.xlsx
+++ b/public/Daily Report_hyunmyung.kim.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,19 +25,19 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>Install New Hazardous Material Pharmacy Building Support</t>
+    <t>ELAC Campus Wide Duct Cleaning</t>
   </si>
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>08/12/2021</t>
+    <t>08/13/2021</t>
   </si>
   <si>
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>FA930115D0011</t>
+    <t>4500289944</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -52,16 +52,19 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
-    <t/>
+    <t>09:32</t>
   </si>
   <si>
     <t>WEATHER</t>
   </si>
   <si>
-    <t>Sunny</t>
+    <t>Snowy</t>
   </si>
   <si>
     <t xml:space="preserve">END TIME </t>
+  </si>
+  <si>
+    <t>09:49</t>
   </si>
   <si>
     <t>CONTRACTOR</t>
@@ -84,6 +87,9 @@
   <si>
     <t xml:space="preserve">HOURS
 /Day</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>TOTAL</t>
@@ -1080,7 +1086,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="12">
-        <v>6082</v>
+        <v>6300</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1112,45 +1118,45 @@
         <v>14</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" ht="36.75" customHeight="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="24"/>
       <c r="C7" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="24"/>
     </row>
     <row r="8" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C8" s="29">
         <v>0</v>
@@ -1159,18 +1165,18 @@
         <v>0</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" ht="21" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C9" s="34">
         <v>0</v>
@@ -1179,52 +1185,28 @@
         <v>0</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="L9" s="37"/>
     </row>
     <row r="10" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="34">
-        <v>0</v>
-      </c>
-      <c r="D10" s="35">
-        <v>0</v>
-      </c>
-      <c r="E10" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="34">
-        <v>0</v>
-      </c>
-      <c r="D11" s="35">
-        <v>0</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>11</v>
-      </c>
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" ht="21" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="32"/>
@@ -1260,11 +1242,11 @@
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" s="39"/>
       <c r="C16" s="40" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="21"/>
@@ -1275,7 +1257,7 @@
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -1286,7 +1268,7 @@
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B18" s="47"/>
       <c r="C18" s="47"/>
@@ -1322,7 +1304,7 @@
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -1333,7 +1315,7 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B23" s="47"/>
       <c r="C23" s="47"/>
@@ -1368,7 +1350,7 @@
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="43" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -1379,7 +1361,7 @@
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>

</xml_diff>